<commit_message>
fixing bug laporan, pembayaran ujian, jenis ujian, revisi database
</commit_message>
<xml_diff>
--- a/uploads/Report Data Siswa .xlsx
+++ b/uploads/Report Data Siswa .xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32">
   <si>
     <t>RINCIAN KEKURANGAN ADMINISTRASI KEUANGAN</t>
   </si>
@@ -43,48 +43,51 @@
     <t>Kelas</t>
   </si>
   <si>
+    <t>XII_ak_A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DPP </t>
+  </si>
+  <si>
+    <t>0,-</t>
+  </si>
+  <si>
+    <t>Kelas 10</t>
+  </si>
+  <si>
+    <t>X_ak_A</t>
+  </si>
+  <si>
+    <t>Biaya SPP</t>
+  </si>
+  <si>
+    <t>UTS Ganjil</t>
+  </si>
+  <si>
+    <t>UAS Ganjil</t>
+  </si>
+  <si>
+    <t>UTS Genap</t>
+  </si>
+  <si>
+    <t>UAS Genap</t>
+  </si>
+  <si>
+    <t>Total Tanggungan Biaya Kelas 10</t>
+  </si>
+  <si>
+    <t>Kelas 11</t>
+  </si>
+  <si>
     <t>XI_ak_A</t>
   </si>
   <si>
-    <t xml:space="preserve">DPP </t>
-  </si>
-  <si>
-    <t>Kelas 10</t>
-  </si>
-  <si>
-    <t>X_ak_A</t>
-  </si>
-  <si>
-    <t>Biaya SPP</t>
-  </si>
-  <si>
-    <t>UTS Ganjil</t>
-  </si>
-  <si>
-    <t>UAS Ganjil</t>
-  </si>
-  <si>
-    <t>UTS Genap</t>
-  </si>
-  <si>
-    <t>UAS Genap</t>
-  </si>
-  <si>
-    <t>Total Tanggungan Biaya Kelas 10</t>
-  </si>
-  <si>
-    <t>Kelas 11</t>
-  </si>
-  <si>
     <t>Total Tanggungan Biaya Kelas 11</t>
   </si>
   <si>
     <t>Kelas 12</t>
   </si>
   <si>
-    <t>0,-</t>
-  </si>
-  <si>
     <t>UNBK</t>
   </si>
   <si>
@@ -95,6 +98,15 @@
   </si>
   <si>
     <t>DPP</t>
+  </si>
+  <si>
+    <t>Total Tanggungan kelas 10</t>
+  </si>
+  <si>
+    <t>Total Tanggungan kelas 11</t>
+  </si>
+  <si>
+    <t>Total Tanggungan kelas 12</t>
   </si>
   <si>
     <t>total Tanggugan Biaya</t>
@@ -464,10 +476,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="B3" sqref="B3:B41"/>
+      <selection activeCell="B3" sqref="B3:B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" defaultColWidth="30" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -528,8 +540,8 @@
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="3">
-        <v>1200000</v>
+      <c r="B9" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -538,7 +550,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" s="3"/>
     </row>
@@ -547,12 +559,12 @@
         <v>7</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" s="3">
         <v>360000</v>
@@ -560,42 +572,42 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" s="3">
-        <v>200000</v>
+        <v>300000</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" s="3">
-        <v>100000</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" s="3">
-        <v>200000</v>
+        <v>300000</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17" s="3">
-        <v>100000</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18" s="3">
-        <v>960000</v>
+        <v>1260000</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -604,7 +616,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" s="3"/>
     </row>
@@ -613,12 +625,12 @@
         <v>7</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B22" s="3">
         <v>360000</v>
@@ -626,42 +638,42 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B23" s="3">
-        <v>200000</v>
+        <v>300000</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B24" s="3">
-        <v>100000</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B25" s="3">
-        <v>200000</v>
+        <v>300000</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B26" s="3">
-        <v>100000</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B27" s="3">
-        <v>960000</v>
+        <v>1260000</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -670,7 +682,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B29" s="3"/>
     </row>
@@ -678,61 +690,65 @@
       <c r="A30" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B30" s="3"/>
+      <c r="B30" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>21</v>
+        <v>13</v>
+      </c>
+      <c r="B31" s="3">
+        <v>360000</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>21</v>
+        <v>15</v>
+      </c>
+      <c r="B33" s="3">
+        <v>150000</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
+      </c>
+      <c r="B35" s="3">
+        <v>150000</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="B36" s="3">
+        <v>625000</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B37" s="3"/>
+        <v>24</v>
+      </c>
+      <c r="B37" s="3">
+        <v>1285000</v>
+      </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="1"/>
@@ -740,24 +756,48 @@
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B39" s="2"/>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B40" s="3">
-        <v>1200000</v>
+        <v>26</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B41" s="3">
-        <v>1920000</v>
+        <v>1260000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B42" s="3">
+        <v>1260000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B43" s="3">
+        <v>1285000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B44" s="3">
+        <v>3805000</v>
       </c>
     </row>
   </sheetData>
@@ -788,10 +828,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="B3" sqref="B3:B41"/>
+      <selection activeCell="B3" sqref="B3:B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" defaultColWidth="30" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -837,7 +877,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -845,7 +885,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -862,7 +902,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" s="3"/>
     </row>
@@ -871,12 +911,12 @@
         <v>7</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" s="3">
         <v>160000</v>
@@ -884,42 +924,42 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>21</v>
+        <v>14</v>
+      </c>
+      <c r="B14" s="3">
+        <v>300000</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>21</v>
+        <v>16</v>
+      </c>
+      <c r="B16" s="3">
+        <v>300000</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="3">
-        <v>100000</v>
+        <v>17</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18" s="3">
-        <v>260000</v>
+        <v>760000</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -928,7 +968,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" s="3"/>
     </row>
@@ -937,12 +977,12 @@
         <v>7</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B22" s="3">
         <v>240000</v>
@@ -950,42 +990,42 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B23" s="3">
-        <v>200000</v>
+        <v>300000</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B24" s="3">
-        <v>100000</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B25" s="3">
-        <v>200000</v>
+        <v>300000</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B26" s="3">
-        <v>100000</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B27" s="3">
-        <v>840000</v>
+        <v>1140000</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -993,95 +1033,45 @@
       <c r="B28" s="2"/>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B29" s="3"/>
+      <c r="A29" s="1"/>
+      <c r="B29" s="2"/>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B30" s="3"/>
+        <v>25</v>
+      </c>
+      <c r="B30" s="2"/>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>21</v>
+        <v>26</v>
+      </c>
+      <c r="B31" s="3">
+        <v>200000</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>21</v>
+        <v>27</v>
+      </c>
+      <c r="B32" s="3">
+        <v>760000</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>21</v>
+        <v>28</v>
+      </c>
+      <c r="B33" s="3">
+        <v>1140000</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B37" s="3"/>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="1"/>
-      <c r="B38" s="2"/>
-    </row>
-    <row r="39" spans="1:2">
-      <c r="A39" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B39" s="2"/>
-    </row>
-    <row r="40" spans="1:2">
-      <c r="A40" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B40" s="3">
-        <v>200000</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
-      <c r="A41" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B41" s="3">
-        <v>1100000</v>
+        <v>30</v>
+      </c>
+      <c r="B34" s="3">
+        <v>2100000</v>
       </c>
     </row>
   </sheetData>
@@ -1091,7 +1081,6 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A29:B29"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>